<commit_message>
modify ray tracing to adopt variable geoid height
</commit_message>
<xml_diff>
--- a/Data/Hydrophone_Position.xlsx
+++ b/Data/Hydrophone_Position.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/testuser/Documents/ONR_RAP/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B7A3C85-2792-7E46-85FF-CB77D4272A1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8024A3E-29A2-E14D-A653-4BB5DC1B8AED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{34ACAB8F-7993-F543-8192-9147B8AA556F}"/>
+    <workbookView xWindow="14460" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{34ACAB8F-7993-F543-8192-9147B8AA556F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6D4CC0-7824-4A44-AE93-E9D1D386245D}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,14 +571,12 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
       <c r="D4" s="2">
-        <v>4.8</v>
+        <v>2.4</v>
       </c>
       <c r="E4" s="5">
         <v>-158.00619</v>
@@ -590,27 +588,25 @@
         <v>4729.92</v>
       </c>
       <c r="H4" s="5">
-        <v>1.63</v>
+        <v>0.61</v>
       </c>
       <c r="I4" s="5">
-        <v>-0.68</v>
+        <v>-0.71699999999999997</v>
       </c>
       <c r="J4" s="5">
-        <v>5.22</v>
+        <v>5.23</v>
       </c>
       <c r="K4" s="5">
-        <v>4735.1400000000003</v>
+        <v>4735.1499999999996</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="2">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
-        <v>4.8</v>
+        <v>2.4</v>
       </c>
       <c r="E5" s="5">
         <v>-158.00619</v>
@@ -621,16 +617,88 @@
       <c r="G5" s="5">
         <v>4729.92</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="E7" s="5">
+        <v>-158.00619</v>
+      </c>
+      <c r="F7" s="5">
+        <v>22.738772000000001</v>
+      </c>
+      <c r="G7" s="5">
+        <v>4729.92</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1.63</v>
+      </c>
+      <c r="I7" s="5">
+        <v>-0.68</v>
+      </c>
+      <c r="J7" s="5">
+        <v>5.22</v>
+      </c>
+      <c r="K7" s="5">
+        <v>4735.1400000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-158.00619</v>
+      </c>
+      <c r="F8" s="5">
+        <v>22.738772000000001</v>
+      </c>
+      <c r="G8" s="5">
+        <v>4729.92</v>
+      </c>
+      <c r="H8" s="5">
         <v>1.01</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I8" s="5">
         <v>-0.84</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J8" s="5">
         <v>4.66</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K8" s="5">
         <v>4734.58</v>
       </c>
     </row>

</xml_diff>